<commit_message>
Add sprint 2 grading
</commit_message>
<xml_diff>
--- a/Equipe203.xlsx
+++ b/Equipe203.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_a9e\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_26b6\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="8_{B3EACF60-D4C3-4F3D-9DF2-0AC70C608458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{75A448FB-3BF8-48CB-A81A-8C1C131D7680}"/>
+  <xr:revisionPtr revIDLastSave="326" documentId="8_{B3EACF60-D4C3-4F3D-9DF2-0AC70C608458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E81C956-EFF2-4D2A-BE2C-7E4A789E7964}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="7" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Old Sudoku" sheetId="1" state="hidden" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Assurance Qualité" sheetId="6" r:id="rId8"/>
     <sheet name="Curling" sheetId="7" state="hidden" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="219">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -365,12 +365,22 @@
     <t>Ne build pas</t>
   </si>
   <si>
+    <t xml:space="preserve">6a001bb246423b18ecdb333091bd32d5c48ab51e
+</t>
+  </si>
+  <si>
     <t>Annuler-refaire</t>
   </si>
   <si>
     <t>Sauvegarder le dessin sur serveur</t>
   </si>
   <si>
+    <t>Les raccourcis habituels de chrome ne sont pas bloqué</t>
+  </si>
+  <si>
+    <t>Lamontagne</t>
+  </si>
+  <si>
     <t>Galerie de dessins</t>
   </si>
   <si>
@@ -383,6 +393,9 @@
     <t>Exporter le dessin</t>
   </si>
   <si>
+    <t>L'exportation exporte une image plus grande que l'image originale (Le background est différent pour la partie ajoutée)</t>
+  </si>
+  <si>
     <t>Outil-Sélection et inversion de sélection</t>
   </si>
   <si>
@@ -392,6 +405,11 @@
     <t>Outil-Efface</t>
   </si>
   <si>
+    <t xml:space="preserve">On ne peut pas supprimer deux éléments qui ne se retrouve pas sur  le même point mais dans la zone de l'efface en même temps.
+Les traits ne sont pas tous effacés si on glisse l'efface rapidement sur les objets.
+</t>
+  </si>
+  <si>
     <t>Outi-Pipette</t>
   </si>
   <si>
@@ -465,6 +483,10 @@
   </si>
   <si>
     <t>Les méthodes seulement utilisées dans le template html peuvent être mises comme protégés au lieu de publiques.</t>
+  </si>
+  <si>
+    <t>-0.25 Tool icon devrait être protected puisqu'il est seulement utilisé dans le html
+-0.25 SidebarColorPickerComponent plusieurs méthodes devraient être protected, car elles sont seulement utilisé dans le html</t>
   </si>
   <si>
     <t>Les attributs de la classe sont initialisés dans le constructeur</t>
@@ -474,6 +496,9 @@
 Pourquoi vous ne créez pas un constructeur pour la classe Color en assignant des paramètres au lieu de toujours les assigner après sa construction</t>
   </si>
   <si>
+    <t>-0.25 ToolLineService incohérence dans l'initialisation des attributs</t>
+  </si>
+  <si>
     <t>Total de la catégorie</t>
   </si>
   <si>
@@ -511,6 +536,10 @@
   </si>
   <si>
     <t>-0.25 create-drawing.component.ts, Validators.max(10000) 10000 devrait être une constante.</t>
+  </si>
+  <si>
+    <t>-0.25 Certaines constantes sont déclarés à l'extérieur des components dans plusieurs fichiers. Exemple : canvasWidth dans HueSlider et AlphaSlider.
+Il faudrait l'importer d'une autre classe au lieu de le redéclarer.</t>
   </si>
   <si>
     <t>Les variables et constantes ont des noms explicites qui respectent les conventions de nommage.</t>
@@ -548,6 +577,9 @@
     <t>-0.25 tool-rectangle.service.ts et tool-line.service.ts - Utilisez une enum pour les noms d'outils plutôt que des string literals</t>
   </si>
   <si>
+    <t>- 0.25 guide-data.ts - vous dupliquez les  noms d'outils plutot que de réutilisez ce qui se trouve dans toolInfo</t>
+  </si>
+  <si>
     <t>Les objets javascript ne sont pas utilisés, des classes ou des interfaces sont utilisés</t>
   </si>
   <si>
@@ -556,6 +588,9 @@
 previewColor.alpha /= 2;</t>
   </si>
   <si>
+    <t>- 0.25 new-drawing.component.ts méthode onSubmit, dimensions anonyme</t>
+  </si>
+  <si>
     <t>Le code est correctement indenté et organisé en groupes logiques.</t>
   </si>
   <si>
@@ -576,6 +611,11 @@
   <si>
     <t>-0.25 panel-settings.component.ts - Méthode getSelectedColor - else inutile (ne fait qu'ajouter du nesting après le return du if)
 -0.25 tool-line.service.ts - Méthode calculateNextPointPosition - retourner directement "mousePosition" dans le premier if réduirait le nesting et les 17 lignes inutiles entre la dernière instruction et le return statement.</t>
+  </si>
+  <si>
+    <t>- 0.25 tool-selection.service.ts méthode updateSelectionOnMouseUp - inverser le if et short circuit
+- 0.25 database.service.ts méthode updateFile - Inverser le if et shortcircuit
+- 0.25 color.service.ts méthode addColor - early return dans le if et retirer le else</t>
   </si>
   <si>
     <t>Le logiciel a des performances acceptables</t>
@@ -3213,9 +3253,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="78" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="77" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="77" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3638,6 +3675,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="102" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="77" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4503,18 +4543,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15"/>
     <row r="2" spans="1:11" ht="15">
-      <c r="C2" s="287" t="s">
+      <c r="C2" s="286" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="287"/>
-      <c r="E2" s="288" t="s">
+      <c r="D2" s="286"/>
+      <c r="E2" s="287" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="288"/>
-      <c r="G2" s="289" t="s">
+      <c r="F2" s="287"/>
+      <c r="G2" s="288" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="289"/>
+      <c r="H2" s="288"/>
     </row>
     <row r="3" spans="1:11" ht="15">
       <c r="A3" s="2"/>
@@ -4795,7 +4835,7 @@
       <c r="F2" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="290" t="s">
+      <c r="G2" s="289" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4808,7 +4848,7 @@
       <c r="D3" s="55"/>
       <c r="E3" s="56"/>
       <c r="F3" s="57"/>
-      <c r="G3" s="290"/>
+      <c r="G3" s="289"/>
     </row>
     <row r="4" spans="1:7" ht="15">
       <c r="A4" s="58" t="s">
@@ -5130,10 +5170,10 @@
       <c r="D27" s="85"/>
       <c r="E27" s="85"/>
       <c r="F27" s="85"/>
-      <c r="H27" s="291" t="s">
+      <c r="H27" s="290" t="s">
         <v>55</v>
       </c>
-      <c r="I27" s="291"/>
+      <c r="I27" s="290"/>
     </row>
     <row r="28" spans="1:9" ht="15">
       <c r="A28" s="52" t="s">
@@ -5488,7 +5528,7 @@
       <c r="F2" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="290" t="s">
+      <c r="G2" s="289" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5501,7 +5541,7 @@
       <c r="D3" s="55"/>
       <c r="E3" s="56"/>
       <c r="F3" s="57"/>
-      <c r="G3" s="290"/>
+      <c r="G3" s="289"/>
     </row>
     <row r="4" spans="1:7" ht="30">
       <c r="A4" s="58" t="s">
@@ -5875,10 +5915,10 @@
       <c r="D31" s="85"/>
       <c r="E31" s="85"/>
       <c r="F31" s="85"/>
-      <c r="H31" s="291" t="s">
+      <c r="H31" s="290" t="s">
         <v>55</v>
       </c>
-      <c r="I31" s="291"/>
+      <c r="I31" s="290"/>
     </row>
     <row r="32" spans="1:9" ht="15">
       <c r="A32" s="52" t="s">
@@ -6215,17 +6255,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7">
-      <c r="A3" s="218"/>
-      <c r="B3" s="266" t="s">
+      <c r="A3" s="217"/>
+      <c r="B3" s="265" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="266" t="s">
+      <c r="C3" s="265" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="266" t="s">
+      <c r="D3" s="265" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="267" t="s">
+      <c r="E3" s="266" t="s">
         <v>77</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -6236,88 +6276,88 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="269">
+      <c r="A4" s="267" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="268">
         <f>(Fonctionnalités!E17)</f>
-        <v>0.96779999999999999</v>
-      </c>
-      <c r="C4" s="270">
+        <v>0.96900000000000008</v>
+      </c>
+      <c r="C4" s="269">
         <f>'Assurance Qualité'!B49</f>
         <v>0.92749999999999999</v>
       </c>
-      <c r="D4" s="270">
+      <c r="D4" s="269">
         <f>AVERAGE(B4:C4) - 0.1*E4</f>
-        <v>0.94764999999999999</v>
-      </c>
-      <c r="F4" s="281">
+        <v>0.94825000000000004</v>
+      </c>
+      <c r="F4" s="280">
         <v>15</v>
       </c>
-      <c r="G4" s="280">
+      <c r="G4" s="279">
         <f>D4*F4</f>
-        <v>14.21475</v>
+        <v>14.223750000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="271" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="272">
+      <c r="A5" s="270" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="271">
         <f>(Fonctionnalités!E39)</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="273">
+        <v>0.97750000000000004</v>
+      </c>
+      <c r="C5" s="272">
         <f>'Assurance Qualité'!D49</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="273">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="D5" s="272">
         <f>AVERAGE(B5:C5) - 0.1*E5</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="281">
-        <v>20</v>
-      </c>
-      <c r="G5" s="280">
+        <v>0.9425</v>
+      </c>
+      <c r="F5" s="280">
+        <v>30</v>
+      </c>
+      <c r="G5" s="279">
         <f t="shared" ref="G5:G7" si="0">D5*F5</f>
-        <v>0</v>
+        <v>28.274999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="274" t="s">
+      <c r="A6" s="273" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="275">
+      <c r="B6" s="274">
         <f>(Fonctionnalités!E58)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="276">
+      <c r="C6" s="275">
         <f>'Assurance Qualité'!F49</f>
         <v>0</v>
       </c>
-      <c r="D6" s="276">
+      <c r="D6" s="275">
         <f>AVERAGE(B6:C6) - 0.1*E6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="281">
+      <c r="F6" s="280">
         <v>25</v>
       </c>
-      <c r="G6" s="280">
+      <c r="G6" s="279">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="277" t="s">
+      <c r="A7" s="276" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="278"/>
-      <c r="C7" s="278"/>
-      <c r="D7" s="282"/>
+      <c r="B7" s="277"/>
+      <c r="C7" s="277"/>
+      <c r="D7" s="281"/>
       <c r="F7" s="2">
-        <v>10</v>
-      </c>
-      <c r="G7" s="280">
+        <v>15</v>
+      </c>
+      <c r="G7" s="279">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6331,8 +6371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A54262-C76A-40FE-9AF3-642EF9B2EA00}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6344,895 +6384,1017 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="300" t="s">
+      <c r="A1" s="299" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="301"/>
-      <c r="C1" s="301"/>
-      <c r="D1" s="301"/>
-      <c r="E1" s="301"/>
-      <c r="F1" s="301"/>
+      <c r="B1" s="300"/>
+      <c r="C1" s="300"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="300"/>
+      <c r="F1" s="300"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="218"/>
-      <c r="B2" s="218"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="219"/>
+      <c r="A2" s="217"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="218"/>
     </row>
     <row r="3" spans="1:7" ht="18.75">
-      <c r="A3" s="300" t="s">
+      <c r="A3" s="299" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="301"/>
-      <c r="C3" s="301"/>
-      <c r="D3" s="301"/>
-      <c r="E3" s="301"/>
-      <c r="F3" s="301"/>
+      <c r="B3" s="300"/>
+      <c r="C3" s="300"/>
+      <c r="D3" s="300"/>
+      <c r="E3" s="300"/>
+      <c r="F3" s="300"/>
     </row>
     <row r="5" spans="1:7" ht="23.25">
-      <c r="A5" s="302" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="302"/>
-      <c r="C5" s="302"/>
-      <c r="D5" s="302"/>
-      <c r="E5" s="302"/>
-      <c r="F5" s="302"/>
+      <c r="A5" s="301" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="301"/>
+      <c r="C5" s="301"/>
+      <c r="D5" s="301"/>
+      <c r="E5" s="301"/>
+      <c r="F5" s="301"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="220" t="s">
+      <c r="A6" s="219" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="303" t="s">
+      <c r="B6" s="302" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="303"/>
-      <c r="D6" s="303"/>
-      <c r="E6" s="303"/>
-      <c r="F6" s="304"/>
+      <c r="C6" s="302"/>
+      <c r="D6" s="302"/>
+      <c r="E6" s="302"/>
+      <c r="F6" s="303"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="221" t="s">
+      <c r="A7" s="220" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="222" t="s">
+      <c r="B7" s="221" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="222" t="s">
+      <c r="C7" s="221" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="222" t="s">
+      <c r="D7" s="221" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="222" t="s">
+      <c r="E7" s="221" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="223" t="s">
+      <c r="F7" s="222" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30">
-      <c r="A8" s="224" t="s">
+      <c r="A8" s="223" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="225">
+      <c r="B8" s="224">
         <v>0.95</v>
       </c>
-      <c r="C8" s="225">
-        <v>1</v>
-      </c>
-      <c r="D8" s="225">
+      <c r="C8" s="224">
+        <v>1</v>
+      </c>
+      <c r="D8" s="224">
         <v>16</v>
       </c>
-      <c r="E8" s="225">
+      <c r="E8" s="224">
         <f t="shared" ref="E8:E13" si="0">B8*C8*D8</f>
         <v>15.2</v>
       </c>
-      <c r="F8" s="226" t="s">
+      <c r="F8" s="225" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="283" t="s">
+      <c r="G8" s="282" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="224" t="s">
+      <c r="A9" s="223" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="225">
-        <v>1</v>
-      </c>
-      <c r="C9" s="225">
-        <v>1</v>
-      </c>
-      <c r="D9" s="225">
+      <c r="B9" s="224">
+        <v>1</v>
+      </c>
+      <c r="C9" s="224">
+        <v>1</v>
+      </c>
+      <c r="D9" s="224">
         <v>8</v>
       </c>
-      <c r="E9" s="225">
+      <c r="E9" s="224">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F9" s="227"/>
-      <c r="G9" s="283" t="s">
+      <c r="F9" s="226"/>
+      <c r="G9" s="282" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="224" t="s">
+      <c r="A10" s="223" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="225">
+      <c r="B10" s="224">
         <v>0.95</v>
       </c>
-      <c r="C10" s="225">
-        <v>1</v>
-      </c>
-      <c r="D10" s="225">
+      <c r="C10" s="224">
+        <v>1</v>
+      </c>
+      <c r="D10" s="224">
         <v>10</v>
       </c>
-      <c r="E10" s="225">
+      <c r="E10" s="224">
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-      <c r="F10" s="227" t="s">
+      <c r="F10" s="226" t="s">
         <v>92</v>
       </c>
-      <c r="G10" s="283" t="s">
+      <c r="G10" s="282" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="224" t="s">
+      <c r="A11" s="223" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="225">
+      <c r="B11" s="224">
         <v>0.95</v>
       </c>
-      <c r="C11" s="225">
-        <v>1</v>
-      </c>
-      <c r="D11" s="225">
+      <c r="C11" s="224">
+        <v>1</v>
+      </c>
+      <c r="D11" s="224">
         <v>12</v>
       </c>
-      <c r="E11" s="225">
+      <c r="E11" s="224">
         <f t="shared" si="0"/>
         <v>11.399999999999999</v>
       </c>
-      <c r="F11" s="226" t="s">
+      <c r="F11" s="225" t="s">
         <v>94</v>
       </c>
-      <c r="G11" s="283" t="s">
+      <c r="G11" s="282" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="224" t="s">
+      <c r="A12" s="223" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="225">
-        <v>1</v>
-      </c>
-      <c r="C12" s="225">
-        <v>1</v>
-      </c>
-      <c r="D12" s="225">
+      <c r="B12" s="224">
+        <v>1</v>
+      </c>
+      <c r="C12" s="224">
+        <v>1</v>
+      </c>
+      <c r="D12" s="224">
         <v>10</v>
       </c>
-      <c r="E12" s="225">
+      <c r="E12" s="224">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F12" s="226"/>
-      <c r="G12" s="283" t="s">
+      <c r="F12" s="225"/>
+      <c r="G12" s="282" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45">
-      <c r="A13" s="224" t="s">
+      <c r="A13" s="223" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="225">
-        <v>0.94</v>
-      </c>
-      <c r="C13" s="225">
-        <v>1</v>
-      </c>
-      <c r="D13" s="225">
+      <c r="B13" s="224">
+        <v>0.95</v>
+      </c>
+      <c r="C13" s="224">
+        <v>1</v>
+      </c>
+      <c r="D13" s="224">
         <v>12</v>
       </c>
-      <c r="E13" s="225">
+      <c r="E13" s="224">
         <f t="shared" si="0"/>
-        <v>11.28</v>
-      </c>
-      <c r="F13" s="226" t="s">
+        <v>11.399999999999999</v>
+      </c>
+      <c r="F13" s="225" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="283" t="s">
+      <c r="G13" s="282" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45">
-      <c r="A14" s="224" t="s">
+      <c r="A14" s="223" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="225">
+      <c r="B14" s="224">
         <v>0.95</v>
       </c>
-      <c r="C14" s="225">
-        <v>1</v>
-      </c>
-      <c r="D14" s="225">
+      <c r="C14" s="224">
+        <v>1</v>
+      </c>
+      <c r="D14" s="224">
         <v>12</v>
       </c>
-      <c r="E14" s="225">
+      <c r="E14" s="224">
         <f t="shared" ref="E14:E16" si="1">B14*C14*D14</f>
         <v>11.399999999999999</v>
       </c>
-      <c r="F14" s="226" t="s">
+      <c r="F14" s="225" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="283" t="s">
+      <c r="G14" s="282" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="224" t="s">
+      <c r="A15" s="223" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="225">
-        <v>1</v>
-      </c>
-      <c r="C15" s="225">
-        <v>1</v>
-      </c>
-      <c r="D15" s="225">
+      <c r="B15" s="224">
+        <v>1</v>
+      </c>
+      <c r="C15" s="224">
+        <v>1</v>
+      </c>
+      <c r="D15" s="224">
         <v>10</v>
       </c>
-      <c r="E15" s="225">
+      <c r="E15" s="224">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="F15" s="227"/>
-      <c r="G15" s="283" t="s">
+      <c r="F15" s="226"/>
+      <c r="G15" s="282" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="224" t="s">
+      <c r="A16" s="223" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="225">
-        <v>1</v>
-      </c>
-      <c r="C16" s="225">
-        <v>1</v>
-      </c>
-      <c r="D16" s="225">
+      <c r="B16" s="224">
+        <v>1</v>
+      </c>
+      <c r="C16" s="224">
+        <v>1</v>
+      </c>
+      <c r="D16" s="224">
         <v>10</v>
       </c>
-      <c r="E16" s="225">
+      <c r="E16" s="224">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="F16" s="227"/>
-      <c r="G16" s="283" t="s">
+      <c r="F16" s="226"/>
+      <c r="G16" s="282" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="60">
-      <c r="A17" s="228" t="s">
+    <row r="17" spans="1:7" ht="60">
+      <c r="A17" s="227" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="305"/>
-      <c r="C17" s="305"/>
-      <c r="D17" s="286">
+      <c r="B17" s="304"/>
+      <c r="C17" s="304"/>
+      <c r="D17" s="285">
         <f>SUM(D8:D16)</f>
         <v>100</v>
       </c>
-      <c r="E17" s="279">
+      <c r="E17" s="278">
         <f>SUM(E8:E16)/D17 - E19*D19 - E18*D18</f>
-        <v>0.96779999999999999</v>
-      </c>
-      <c r="F17" s="285" t="s">
+        <v>0.96900000000000008</v>
+      </c>
+      <c r="F17" s="284" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="229" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" s="228" t="s">
         <v>105</v>
       </c>
-      <c r="D18" s="230">
+      <c r="D18" s="229">
         <v>0.15</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="229" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" s="228" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="230">
+      <c r="D19" s="229">
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="23.25">
-      <c r="A20" s="306" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="307"/>
-      <c r="C20" s="307"/>
-      <c r="D20" s="307"/>
-      <c r="E20" s="307"/>
-      <c r="F20" s="308"/>
-    </row>
-    <row r="21" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A21" s="239" t="s">
+    <row r="20" spans="1:7" ht="23.25">
+      <c r="A20" s="305" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="306"/>
+      <c r="C20" s="306"/>
+      <c r="D20" s="306"/>
+      <c r="E20" s="306"/>
+      <c r="F20" s="307"/>
+    </row>
+    <row r="21" spans="1:7" ht="25.5" customHeight="1">
+      <c r="A21" s="238" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="292"/>
-      <c r="C21" s="293"/>
-      <c r="D21" s="293"/>
-      <c r="E21" s="293"/>
-      <c r="F21" s="294"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="239" t="s">
+      <c r="B21" s="291" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="292"/>
+      <c r="D21" s="292"/>
+      <c r="E21" s="292"/>
+      <c r="F21" s="293"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="238" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="231" t="s">
+      <c r="B22" s="230" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="231" t="s">
+      <c r="C22" s="230" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="231" t="s">
+      <c r="D22" s="230" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="231" t="s">
+      <c r="E22" s="230" t="s">
         <v>84</v>
       </c>
-      <c r="F22" s="240" t="s">
+      <c r="F22" s="239" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="239" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" s="253"/>
-      <c r="C23" s="253"/>
-      <c r="D23" s="231">
+    <row r="23" spans="1:7">
+      <c r="A23" s="238" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="252">
+        <v>1</v>
+      </c>
+      <c r="C23" s="252">
+        <v>1</v>
+      </c>
+      <c r="D23" s="230">
         <v>12</v>
       </c>
-      <c r="E23" s="231">
+      <c r="E23" s="230">
         <f>B23*C23*D23</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="240"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="239" t="s">
-        <v>108</v>
-      </c>
-      <c r="B24" s="253"/>
-      <c r="C24" s="253"/>
-      <c r="D24" s="231">
+        <v>12</v>
+      </c>
+      <c r="F23" s="239"/>
+      <c r="G23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="238" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="252">
+        <v>1</v>
+      </c>
+      <c r="C24" s="252">
+        <v>1</v>
+      </c>
+      <c r="D24" s="230">
         <v>8</v>
       </c>
-      <c r="E24" s="231">
+      <c r="E24" s="230">
         <f>B24*C24*D24</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="240"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="239" t="s">
-        <v>109</v>
-      </c>
-      <c r="B25" s="253"/>
-      <c r="C25" s="253"/>
-      <c r="D25" s="231">
         <v>8</v>
       </c>
-      <c r="E25" s="231">
+      <c r="F24" s="239" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="238" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="252">
+        <v>1</v>
+      </c>
+      <c r="C25" s="252">
+        <v>1</v>
+      </c>
+      <c r="D25" s="230">
+        <v>8</v>
+      </c>
+      <c r="E25" s="230">
         <f>B25*C25*D25</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="240"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="239" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="239" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="253"/>
-      <c r="C26" s="253"/>
-      <c r="D26" s="231">
+      <c r="G25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="238" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="252">
+        <v>1</v>
+      </c>
+      <c r="C26" s="252">
+        <v>1</v>
+      </c>
+      <c r="D26" s="230">
         <v>4</v>
       </c>
-      <c r="E26" s="231">
+      <c r="E26" s="230">
         <f>B26*C26*D26</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="240"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="239" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="239"/>
+      <c r="G26" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="253"/>
-      <c r="C27" s="253"/>
-      <c r="D27" s="231">
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="238" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="252">
+        <v>1</v>
+      </c>
+      <c r="C27" s="252">
+        <v>1</v>
+      </c>
+      <c r="D27" s="230">
         <v>5</v>
       </c>
-      <c r="E27" s="231">
+      <c r="E27" s="230">
         <f>B27*C27*D27</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="240"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="239" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" s="253"/>
-      <c r="C28" s="253"/>
-      <c r="D28" s="231">
         <v>5</v>
       </c>
-      <c r="E28" s="231">
+      <c r="F27" s="239"/>
+      <c r="G27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30">
+      <c r="A28" s="238" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="252">
+        <v>0.95</v>
+      </c>
+      <c r="C28" s="252">
+        <v>1</v>
+      </c>
+      <c r="D28" s="230">
+        <v>5</v>
+      </c>
+      <c r="E28" s="230">
         <f t="shared" ref="E28:E38" si="2">B28*C28*D28</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="240"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="239" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="253"/>
-      <c r="C29" s="253"/>
-      <c r="D29" s="231">
+        <v>4.75</v>
+      </c>
+      <c r="F28" s="239" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="238" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="252">
+        <v>1</v>
+      </c>
+      <c r="C29" s="252">
+        <v>1</v>
+      </c>
+      <c r="D29" s="230">
         <v>14</v>
       </c>
-      <c r="E29" s="231">
+      <c r="E29" s="230">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="240"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="239" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="253"/>
-      <c r="C30" s="253"/>
-      <c r="D30" s="231">
+        <v>14</v>
+      </c>
+      <c r="F29" s="239"/>
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="238" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="252">
+        <v>1</v>
+      </c>
+      <c r="C30" s="252">
+        <v>1</v>
+      </c>
+      <c r="D30" s="230">
         <v>6</v>
       </c>
-      <c r="E30" s="231">
+      <c r="E30" s="230">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="240"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="239" t="s">
-        <v>115</v>
-      </c>
-      <c r="B31" s="253"/>
-      <c r="C31" s="253"/>
-      <c r="D31" s="231">
+        <v>6</v>
+      </c>
+      <c r="F30" s="239"/>
+      <c r="G30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="60">
+      <c r="A31" s="238" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="252">
+        <v>0.75</v>
+      </c>
+      <c r="C31" s="252">
+        <v>1</v>
+      </c>
+      <c r="D31" s="230">
         <v>8</v>
       </c>
-      <c r="E31" s="231">
+      <c r="E31" s="230">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="240"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="239" t="s">
-        <v>116</v>
-      </c>
-      <c r="B32" s="253"/>
-      <c r="C32" s="253"/>
-      <c r="D32" s="231">
+        <v>6</v>
+      </c>
+      <c r="F31" s="239" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="238" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="252">
+        <v>1</v>
+      </c>
+      <c r="C32" s="252">
+        <v>1</v>
+      </c>
+      <c r="D32" s="230">
         <v>4</v>
       </c>
-      <c r="E32" s="231">
+      <c r="E32" s="230">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="240"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="239" t="s">
-        <v>117</v>
-      </c>
-      <c r="B33" s="253"/>
-      <c r="C33" s="253"/>
-      <c r="D33" s="231">
         <v>4</v>
       </c>
-      <c r="E33" s="231">
+      <c r="F32" s="239"/>
+      <c r="G32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="238" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="252">
+        <v>1</v>
+      </c>
+      <c r="C33" s="252">
+        <v>1</v>
+      </c>
+      <c r="D33" s="230">
+        <v>4</v>
+      </c>
+      <c r="E33" s="230">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="240"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="252" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" s="253"/>
-      <c r="C34" s="253"/>
-      <c r="D34" s="253">
+        <v>4</v>
+      </c>
+      <c r="F33" s="239"/>
+      <c r="G33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="251" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="252">
+        <v>1</v>
+      </c>
+      <c r="C34" s="252">
+        <v>1</v>
+      </c>
+      <c r="D34" s="252">
         <v>6</v>
       </c>
-      <c r="E34" s="231">
+      <c r="E34" s="230">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="254"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="252" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="253"/>
-      <c r="C35" s="253"/>
-      <c r="D35" s="253">
         <v>6</v>
       </c>
-      <c r="E35" s="231">
+      <c r="F34" s="253"/>
+      <c r="G34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="251" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="252">
+        <v>1</v>
+      </c>
+      <c r="C35" s="252">
+        <v>1</v>
+      </c>
+      <c r="D35" s="252">
+        <v>6</v>
+      </c>
+      <c r="E35" s="230">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="254"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="252" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="253"/>
-      <c r="C36" s="253"/>
-      <c r="D36" s="253">
+        <v>6</v>
+      </c>
+      <c r="F35" s="253"/>
+      <c r="G35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="251" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="252">
+        <v>1</v>
+      </c>
+      <c r="C36" s="252">
+        <v>1</v>
+      </c>
+      <c r="D36" s="252">
         <v>4</v>
       </c>
-      <c r="E36" s="231">
+      <c r="E36" s="230">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="254"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="252" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" s="253"/>
-      <c r="C37" s="253"/>
-      <c r="D37" s="253">
         <v>4</v>
       </c>
-      <c r="E37" s="231">
+      <c r="F36" s="253"/>
+      <c r="G36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="251" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" s="252">
+        <v>1</v>
+      </c>
+      <c r="C37" s="252">
+        <v>1</v>
+      </c>
+      <c r="D37" s="252">
+        <v>4</v>
+      </c>
+      <c r="E37" s="230">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="254"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="252" t="s">
-        <v>122</v>
-      </c>
-      <c r="B38" s="253"/>
-      <c r="C38" s="253"/>
-      <c r="D38" s="253">
+        <v>4</v>
+      </c>
+      <c r="F37" s="253"/>
+      <c r="G37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="251" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" s="252">
+        <v>1</v>
+      </c>
+      <c r="C38" s="252">
+        <v>1</v>
+      </c>
+      <c r="D38" s="252">
         <v>2</v>
       </c>
-      <c r="E38" s="231">
+      <c r="E38" s="230">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="254"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="241" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="253"/>
+      <c r="G38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="240" t="s">
         <v>103</v>
       </c>
-      <c r="B39" s="242"/>
-      <c r="C39" s="263"/>
-      <c r="D39" s="263">
+      <c r="B39" s="241"/>
+      <c r="C39" s="262"/>
+      <c r="D39" s="262">
         <f>SUM(D23:D38)</f>
         <v>100</v>
       </c>
-      <c r="E39" s="243">
+      <c r="E39" s="242">
         <f>SUM(E23:E38)/D39 -E40*D40 -E41*D41-E42*D42</f>
-        <v>0</v>
-      </c>
-      <c r="F39" s="244"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="232" t="s">
+        <v>0.97750000000000004</v>
+      </c>
+      <c r="F39" s="243"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="231" t="s">
         <v>105</v>
       </c>
-      <c r="C40" s="265"/>
-      <c r="D40" s="264">
+      <c r="C40" s="264"/>
+      <c r="D40" s="263">
         <v>0.15</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="232" t="s">
+    <row r="41" spans="1:7">
+      <c r="A41" s="231" t="s">
         <v>106</v>
       </c>
-      <c r="D41" s="233">
+      <c r="D41" s="232">
         <v>0.2</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="232" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" s="234">
+    <row r="42" spans="1:7">
+      <c r="A42" s="231" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" s="233">
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="23.25">
-      <c r="A43" s="295" t="s">
+    <row r="43" spans="1:7" ht="23.25">
+      <c r="A43" s="294" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="296"/>
-      <c r="C43" s="296"/>
-      <c r="D43" s="296"/>
-      <c r="E43" s="296"/>
-      <c r="F43" s="297"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="245" t="s">
+      <c r="B43" s="295"/>
+      <c r="C43" s="295"/>
+      <c r="D43" s="295"/>
+      <c r="E43" s="295"/>
+      <c r="F43" s="296"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="244" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="298"/>
-      <c r="C44" s="298"/>
-      <c r="D44" s="298"/>
-      <c r="E44" s="298"/>
-      <c r="F44" s="299"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="246" t="s">
+      <c r="B44" s="297"/>
+      <c r="C44" s="297"/>
+      <c r="D44" s="297"/>
+      <c r="E44" s="297"/>
+      <c r="F44" s="298"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="245" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="235" t="s">
+      <c r="B45" s="234" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="235" t="s">
+      <c r="C45" s="234" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="235" t="s">
+      <c r="D45" s="234" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="235" t="s">
+      <c r="E45" s="234" t="s">
         <v>84</v>
       </c>
-      <c r="F45" s="247" t="s">
+      <c r="F45" s="246" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="248" t="s">
-        <v>124</v>
-      </c>
-      <c r="B46" s="236"/>
-      <c r="C46" s="236"/>
-      <c r="D46" s="236">
+    <row r="46" spans="1:7">
+      <c r="A46" s="247" t="s">
+        <v>129</v>
+      </c>
+      <c r="B46" s="235"/>
+      <c r="C46" s="235"/>
+      <c r="D46" s="235">
         <v>5</v>
       </c>
-      <c r="E46" s="236">
+      <c r="E46" s="235">
         <f t="shared" ref="E46:E52" si="3">B46*C46*D46</f>
         <v>0</v>
       </c>
-      <c r="F46" s="247"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="248" t="s">
-        <v>125</v>
-      </c>
-      <c r="B47" s="236"/>
-      <c r="C47" s="236"/>
-      <c r="D47" s="236">
+      <c r="F46" s="246"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="247" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="235"/>
+      <c r="C47" s="235"/>
+      <c r="D47" s="235">
         <v>10</v>
       </c>
-      <c r="E47" s="236">
+      <c r="E47" s="235">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F47" s="249"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="248" t="s">
-        <v>126</v>
-      </c>
-      <c r="B48" s="236"/>
-      <c r="C48" s="236"/>
-      <c r="D48" s="236">
+      <c r="F47" s="248"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="247" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="235"/>
+      <c r="C48" s="235"/>
+      <c r="D48" s="235">
         <v>8</v>
       </c>
-      <c r="E48" s="236">
+      <c r="E48" s="235">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F48" s="247"/>
+      <c r="F48" s="246"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="248" t="s">
+      <c r="A49" s="247" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" s="235"/>
+      <c r="C49" s="235"/>
+      <c r="D49" s="235">
+        <v>6</v>
+      </c>
+      <c r="E49" s="235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="248"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="247" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" s="235"/>
+      <c r="C50" s="235"/>
+      <c r="D50" s="235">
+        <v>6</v>
+      </c>
+      <c r="E50" s="235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="246"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="247" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" s="235"/>
+      <c r="C51" s="235"/>
+      <c r="D51" s="235">
+        <v>15</v>
+      </c>
+      <c r="E51" s="235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="246"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="247" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52" s="235"/>
+      <c r="C52" s="235"/>
+      <c r="D52" s="235">
+        <v>8</v>
+      </c>
+      <c r="E52" s="235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="246"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="247" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53" s="255"/>
+      <c r="C53" s="255"/>
+      <c r="D53" s="235">
+        <v>12</v>
+      </c>
+      <c r="E53" s="235">
+        <f t="shared" ref="E53:E57" si="4">B53*C53*D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="246"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="259" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" s="257"/>
+      <c r="C54" s="257"/>
+      <c r="D54" s="254">
+        <v>12</v>
+      </c>
+      <c r="E54" s="235">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="256"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="259" t="s">
+        <v>138</v>
+      </c>
+      <c r="B55" s="257"/>
+      <c r="C55" s="257"/>
+      <c r="D55" s="254">
+        <v>12</v>
+      </c>
+      <c r="E55" s="235">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="256"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="259" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" s="257"/>
+      <c r="C56" s="257"/>
+      <c r="D56" s="254">
+        <v>4</v>
+      </c>
+      <c r="E56" s="235">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="256"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="259" t="s">
         <v>127</v>
       </c>
-      <c r="B49" s="236"/>
-      <c r="C49" s="236"/>
-      <c r="D49" s="236">
-        <v>6</v>
-      </c>
-      <c r="E49" s="236">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="249"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="248" t="s">
-        <v>128</v>
-      </c>
-      <c r="B50" s="236"/>
-      <c r="C50" s="236"/>
-      <c r="D50" s="236">
-        <v>6</v>
-      </c>
-      <c r="E50" s="236">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F50" s="247"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="248" t="s">
-        <v>129</v>
-      </c>
-      <c r="B51" s="236"/>
-      <c r="C51" s="236"/>
-      <c r="D51" s="236">
-        <v>15</v>
-      </c>
-      <c r="E51" s="236">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F51" s="247"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="248" t="s">
-        <v>130</v>
-      </c>
-      <c r="B52" s="236"/>
-      <c r="C52" s="236"/>
-      <c r="D52" s="236">
-        <v>8</v>
-      </c>
-      <c r="E52" s="236">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F52" s="247"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="248" t="s">
-        <v>131</v>
-      </c>
-      <c r="B53" s="256"/>
-      <c r="C53" s="256"/>
-      <c r="D53" s="236">
-        <v>12</v>
-      </c>
-      <c r="E53" s="236">
-        <f t="shared" ref="E53:E57" si="4">B53*C53*D53</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="247"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="260" t="s">
-        <v>132</v>
-      </c>
-      <c r="B54" s="258"/>
-      <c r="C54" s="258"/>
-      <c r="D54" s="255">
-        <v>12</v>
-      </c>
-      <c r="E54" s="236">
+      <c r="B57" s="257"/>
+      <c r="C57" s="257"/>
+      <c r="D57" s="254">
+        <v>2</v>
+      </c>
+      <c r="E57" s="235">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F54" s="257"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="260" t="s">
-        <v>133</v>
-      </c>
-      <c r="B55" s="258"/>
-      <c r="C55" s="258"/>
-      <c r="D55" s="255">
-        <v>12</v>
-      </c>
-      <c r="E55" s="236">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F55" s="257"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="260" t="s">
-        <v>134</v>
-      </c>
-      <c r="B56" s="258"/>
-      <c r="C56" s="258"/>
-      <c r="D56" s="255">
-        <v>4</v>
-      </c>
-      <c r="E56" s="236">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F56" s="257"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="260" t="s">
-        <v>122</v>
-      </c>
-      <c r="B57" s="258"/>
-      <c r="C57" s="258"/>
-      <c r="D57" s="255">
-        <v>2</v>
-      </c>
-      <c r="E57" s="236">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F57" s="257"/>
+      <c r="F57" s="256"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="261" t="s">
+      <c r="A58" s="260" t="s">
         <v>103</v>
       </c>
-      <c r="B58" s="259"/>
-      <c r="C58" s="259"/>
-      <c r="D58" s="262">
+      <c r="B58" s="258"/>
+      <c r="C58" s="258"/>
+      <c r="D58" s="261">
         <f>SUM(D46:D57)</f>
         <v>100</v>
       </c>
-      <c r="E58" s="250">
+      <c r="E58" s="249">
         <f>SUM(E46:E57)/D58 - D59*E59  - D60*E60 - D61*E61</f>
         <v>0</v>
       </c>
-      <c r="F58" s="251"/>
+      <c r="F58" s="250"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="237" t="s">
+      <c r="A59" s="236" t="s">
         <v>105</v>
       </c>
-      <c r="D59" s="233">
+      <c r="D59" s="232">
         <v>0.15</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="237" t="s">
+      <c r="A60" s="236" t="s">
         <v>106</v>
       </c>
-      <c r="D60" s="233">
+      <c r="D60" s="232">
         <v>0.2</v>
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="238" t="s">
-        <v>123</v>
-      </c>
-      <c r="D61" s="234">
+      <c r="A61" s="237" t="s">
+        <v>128</v>
+      </c>
+      <c r="D61" s="233">
         <v>0.05</v>
       </c>
     </row>
@@ -7269,8 +7431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7279,41 +7441,43 @@
     <col min="2" max="3" width="12.7109375" style="1" customWidth="1"/>
     <col min="4" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="104.7109375" customWidth="1"/>
-    <col min="11" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="1025" width="11.42578125"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="47" customWidth="1"/>
+    <col min="12" max="12" width="32.140625" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" customWidth="1"/>
+    <col min="14" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A1" s="309" t="s">
+      <c r="A1" s="308" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="310"/>
-      <c r="C1" s="310"/>
-      <c r="D1" s="310"/>
-      <c r="E1" s="310"/>
-      <c r="F1" s="310"/>
-      <c r="G1" s="311"/>
-      <c r="H1" s="217"/>
-      <c r="I1" s="217"/>
+      <c r="B1" s="309"/>
+      <c r="C1" s="309"/>
+      <c r="D1" s="309"/>
+      <c r="E1" s="309"/>
+      <c r="F1" s="309"/>
+      <c r="G1" s="310"/>
+      <c r="H1" s="216"/>
+      <c r="I1" s="216"/>
     </row>
     <row r="2" spans="1:13" ht="15">
-      <c r="H2" s="200"/>
-      <c r="I2" s="200"/>
+      <c r="H2" s="199"/>
+      <c r="I2" s="199"/>
     </row>
     <row r="3" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A3" s="312" t="s">
+      <c r="A3" s="311" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="313"/>
-      <c r="C3" s="313"/>
-      <c r="D3" s="313"/>
-      <c r="E3" s="313"/>
-      <c r="F3" s="313"/>
-      <c r="G3" s="314"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
+      <c r="B3" s="312"/>
+      <c r="C3" s="312"/>
+      <c r="D3" s="312"/>
+      <c r="E3" s="312"/>
+      <c r="F3" s="312"/>
+      <c r="G3" s="313"/>
+      <c r="H3" s="195"/>
+      <c r="I3" s="195"/>
     </row>
     <row r="4" spans="1:13" ht="18.75">
       <c r="A4" s="145"/>
@@ -7327,51 +7491,51 @@
       <c r="I4" s="146"/>
     </row>
     <row r="5" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A5" s="320" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="322" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="322"/>
-      <c r="D5" s="323" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="323"/>
-      <c r="F5" s="324" t="s">
+      <c r="A5" s="319" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="321" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="321"/>
+      <c r="D5" s="322" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="322"/>
+      <c r="F5" s="323" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="325"/>
-      <c r="H5" s="195"/>
-      <c r="I5" s="195"/>
-      <c r="J5" s="315" t="s">
+      <c r="G5" s="324"/>
+      <c r="H5" s="194"/>
+      <c r="I5" s="194"/>
+      <c r="J5" s="314" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="316"/>
-      <c r="L5" s="316"/>
+      <c r="K5" s="315"/>
+      <c r="L5" s="315"/>
     </row>
     <row r="6" spans="1:13" ht="18.75">
-      <c r="A6" s="321"/>
+      <c r="A6" s="320"/>
       <c r="B6" s="147" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="148" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D6" s="149" t="s">
         <v>48</v>
       </c>
       <c r="E6" s="150" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F6" s="151" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="202" t="s">
-        <v>136</v>
-      </c>
-      <c r="H6" s="195"/>
-      <c r="I6" s="195"/>
+      <c r="G6" s="201" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="194"/>
+      <c r="I6" s="194"/>
       <c r="J6" s="152" t="s">
         <v>0</v>
       </c>
@@ -7384,23 +7548,23 @@
       <c r="M6" s="152"/>
     </row>
     <row r="7" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A7" s="317" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="318"/>
-      <c r="C7" s="318"/>
-      <c r="D7" s="318"/>
-      <c r="E7" s="318"/>
-      <c r="F7" s="318"/>
-      <c r="G7" s="319"/>
-      <c r="H7" s="196" t="s">
-        <v>90</v>
-      </c>
-      <c r="I7" s="196"/>
+      <c r="A7" s="316" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="317"/>
+      <c r="C7" s="317"/>
+      <c r="D7" s="317"/>
+      <c r="E7" s="317"/>
+      <c r="F7" s="317"/>
+      <c r="G7" s="318"/>
+      <c r="H7" s="195" t="s">
+        <v>96</v>
+      </c>
+      <c r="I7" s="195"/>
     </row>
     <row r="8" spans="1:13" ht="60">
-      <c r="A8" s="203" t="s">
-        <v>138</v>
+      <c r="A8" s="202" t="s">
+        <v>143</v>
       </c>
       <c r="B8" s="153">
         <v>1</v>
@@ -7408,20 +7572,22 @@
       <c r="C8" s="154">
         <v>8</v>
       </c>
-      <c r="D8" s="155"/>
+      <c r="D8" s="155">
+        <v>1</v>
+      </c>
       <c r="E8" s="156">
         <v>8</v>
       </c>
       <c r="F8" s="157"/>
-      <c r="G8" s="204">
+      <c r="G8" s="203">
         <v>8</v>
       </c>
-      <c r="H8" s="197"/>
-      <c r="I8" s="197"/>
-    </row>
-    <row r="9" spans="1:13" ht="21" customHeight="1">
-      <c r="A9" s="205" t="s">
-        <v>139</v>
+      <c r="H8" s="196"/>
+      <c r="I8" s="196"/>
+    </row>
+    <row r="9" spans="1:13" ht="120">
+      <c r="A9" s="204" t="s">
+        <v>144</v>
       </c>
       <c r="B9" s="158">
         <v>1</v>
@@ -7429,23 +7595,28 @@
       <c r="C9" s="159">
         <v>2</v>
       </c>
-      <c r="D9" s="160"/>
+      <c r="D9" s="160">
+        <v>0.5</v>
+      </c>
       <c r="E9" s="161">
         <v>2</v>
       </c>
       <c r="F9" s="162"/>
-      <c r="G9" s="206">
+      <c r="G9" s="205">
         <v>2</v>
       </c>
-      <c r="H9" s="197"/>
-      <c r="I9" s="197"/>
+      <c r="H9" s="196"/>
+      <c r="I9" s="196"/>
       <c r="J9" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="60">
-      <c r="A10" s="207" t="s">
-        <v>141</v>
+        <v>145</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="48.75" customHeight="1">
+      <c r="A10" s="206" t="s">
+        <v>147</v>
       </c>
       <c r="B10" s="158">
         <v>0.75</v>
@@ -7453,25 +7624,30 @@
       <c r="C10" s="163">
         <v>4</v>
       </c>
-      <c r="D10" s="160"/>
+      <c r="D10" s="160">
+        <v>0.75</v>
+      </c>
       <c r="E10" s="164">
         <v>4</v>
       </c>
       <c r="F10" s="162"/>
-      <c r="G10" s="208">
+      <c r="G10" s="207">
         <v>4</v>
       </c>
-      <c r="H10" s="197"/>
-      <c r="I10" s="197"/>
+      <c r="H10" s="196"/>
+      <c r="I10" s="196"/>
       <c r="J10" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
+      </c>
+      <c r="K10" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15">
-      <c r="A11" s="209" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11" s="187">
+      <c r="A11" s="208" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="186">
         <f>SUMPRODUCT(B8:B10,C8:C10)</f>
         <v>13</v>
       </c>
@@ -7479,9 +7655,9 @@
         <f>SUM(C8:C10)</f>
         <v>14</v>
       </c>
-      <c r="D11" s="188">
+      <c r="D11" s="187">
         <f>SUMPRODUCT(D8:D10,E8:E10)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E11" s="166">
         <f>SUM(E8:E10)</f>
@@ -7491,31 +7667,31 @@
         <f>SUMPRODUCT(F8:F10,G8:G10)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="208">
+      <c r="G11" s="207">
         <f>SUM(G8:G10)</f>
         <v>14</v>
       </c>
-      <c r="H11" s="197"/>
-      <c r="I11" s="197"/>
+      <c r="H11" s="196"/>
+      <c r="I11" s="196"/>
     </row>
     <row r="12" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A12" s="317" t="s">
-        <v>144</v>
-      </c>
-      <c r="B12" s="318"/>
-      <c r="C12" s="318"/>
-      <c r="D12" s="318"/>
-      <c r="E12" s="318"/>
-      <c r="F12" s="318"/>
-      <c r="G12" s="319"/>
-      <c r="H12" s="196" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" s="196"/>
+      <c r="A12" s="316" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="317"/>
+      <c r="C12" s="317"/>
+      <c r="D12" s="317"/>
+      <c r="E12" s="317"/>
+      <c r="F12" s="317"/>
+      <c r="G12" s="318"/>
+      <c r="H12" s="195" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" s="195"/>
     </row>
     <row r="13" spans="1:13" ht="30">
-      <c r="A13" s="203" t="s">
-        <v>145</v>
+      <c r="A13" s="202" t="s">
+        <v>152</v>
       </c>
       <c r="B13" s="168">
         <v>1</v>
@@ -7523,20 +7699,22 @@
       <c r="C13" s="159">
         <v>6</v>
       </c>
-      <c r="D13" s="169"/>
+      <c r="D13" s="169">
+        <v>1</v>
+      </c>
       <c r="E13" s="161">
         <v>6</v>
       </c>
       <c r="F13" s="170"/>
-      <c r="G13" s="204">
+      <c r="G13" s="203">
         <v>6</v>
       </c>
-      <c r="H13" s="198"/>
-      <c r="I13" s="197"/>
+      <c r="H13" s="197"/>
+      <c r="I13" s="196"/>
     </row>
     <row r="14" spans="1:13" ht="30">
-      <c r="A14" s="205" t="s">
-        <v>146</v>
+      <c r="A14" s="204" t="s">
+        <v>153</v>
       </c>
       <c r="B14" s="171">
         <v>1</v>
@@ -7544,20 +7722,22 @@
       <c r="C14" s="159">
         <v>2</v>
       </c>
-      <c r="D14" s="172"/>
+      <c r="D14" s="172">
+        <v>1</v>
+      </c>
       <c r="E14" s="161">
         <v>2</v>
       </c>
       <c r="F14" s="173"/>
-      <c r="G14" s="206">
+      <c r="G14" s="205">
         <v>2</v>
       </c>
-      <c r="H14" s="198"/>
-      <c r="I14" s="197"/>
+      <c r="H14" s="197"/>
+      <c r="I14" s="196"/>
     </row>
     <row r="15" spans="1:13" ht="15">
-      <c r="A15" s="205" t="s">
-        <v>147</v>
+      <c r="A15" s="204" t="s">
+        <v>154</v>
       </c>
       <c r="B15" s="171">
         <v>1</v>
@@ -7565,20 +7745,22 @@
       <c r="C15" s="159">
         <v>3</v>
       </c>
-      <c r="D15" s="172"/>
+      <c r="D15" s="172">
+        <v>1</v>
+      </c>
       <c r="E15" s="161">
         <v>3</v>
       </c>
       <c r="F15" s="173"/>
-      <c r="G15" s="206">
+      <c r="G15" s="205">
         <v>3</v>
       </c>
-      <c r="H15" s="198"/>
-      <c r="I15" s="197"/>
+      <c r="H15" s="197"/>
+      <c r="I15" s="196"/>
     </row>
     <row r="16" spans="1:13" ht="47.25" customHeight="1">
-      <c r="A16" s="207" t="s">
-        <v>148</v>
+      <c r="A16" s="206" t="s">
+        <v>155</v>
       </c>
       <c r="B16" s="174">
         <v>1</v>
@@ -7586,25 +7768,27 @@
       <c r="C16" s="159">
         <v>2</v>
       </c>
-      <c r="D16" s="175"/>
+      <c r="D16" s="175">
+        <v>1</v>
+      </c>
       <c r="E16" s="161">
         <v>2</v>
       </c>
       <c r="F16" s="173"/>
-      <c r="G16" s="206">
+      <c r="G16" s="205">
         <v>2</v>
       </c>
-      <c r="H16" s="198"/>
-      <c r="I16" s="197"/>
+      <c r="H16" s="197"/>
+      <c r="I16" s="196"/>
       <c r="J16" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15">
-      <c r="A17" s="209" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17" s="187">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15">
+      <c r="A17" s="208" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="186">
         <f>SUMPRODUCT(B13:B16,C13:C16)</f>
         <v>13</v>
       </c>
@@ -7612,9 +7796,9 @@
         <f>SUM(C13:C16)</f>
         <v>13</v>
       </c>
-      <c r="D17" s="188">
+      <c r="D17" s="187">
         <f>SUMPRODUCT(D13:D16,E13:E16)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E17" s="164">
         <f>SUM(E13:E16)</f>
@@ -7624,31 +7808,31 @@
         <f>SUMPRODUCT(F13:F16,G13:G16)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="208">
+      <c r="G17" s="207">
         <f>SUM(G13:G16)</f>
         <v>13</v>
       </c>
-      <c r="H17" s="198"/>
-      <c r="I17" s="197"/>
-    </row>
-    <row r="18" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A18" s="317" t="s">
-        <v>150</v>
-      </c>
-      <c r="B18" s="318"/>
-      <c r="C18" s="318"/>
-      <c r="D18" s="318"/>
-      <c r="E18" s="318"/>
-      <c r="F18" s="318"/>
-      <c r="G18" s="319"/>
-      <c r="H18" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="I18" s="196"/>
-    </row>
-    <row r="19" spans="1:10" ht="15">
-      <c r="A19" s="205" t="s">
-        <v>151</v>
+      <c r="H17" s="197"/>
+      <c r="I17" s="196"/>
+    </row>
+    <row r="18" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A18" s="316" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" s="317"/>
+      <c r="C18" s="317"/>
+      <c r="D18" s="317"/>
+      <c r="E18" s="317"/>
+      <c r="F18" s="317"/>
+      <c r="G18" s="318"/>
+      <c r="H18" s="195" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="195"/>
+    </row>
+    <row r="19" spans="1:11" ht="15">
+      <c r="A19" s="204" t="s">
+        <v>158</v>
       </c>
       <c r="B19" s="158">
         <v>1</v>
@@ -7656,20 +7840,22 @@
       <c r="C19" s="159">
         <v>2</v>
       </c>
-      <c r="D19" s="160"/>
+      <c r="D19" s="160">
+        <v>1</v>
+      </c>
       <c r="E19" s="161">
         <v>2</v>
       </c>
       <c r="F19" s="162"/>
-      <c r="G19" s="206">
+      <c r="G19" s="205">
         <v>2</v>
       </c>
-      <c r="H19" s="198"/>
-      <c r="I19" s="197"/>
-    </row>
-    <row r="20" spans="1:10" ht="15">
-      <c r="A20" s="207" t="s">
-        <v>152</v>
+      <c r="H19" s="197"/>
+      <c r="I19" s="196"/>
+    </row>
+    <row r="20" spans="1:11" ht="15">
+      <c r="A20" s="206" t="s">
+        <v>159</v>
       </c>
       <c r="B20" s="158">
         <v>1</v>
@@ -7677,22 +7863,24 @@
       <c r="C20" s="163">
         <v>2</v>
       </c>
-      <c r="D20" s="160"/>
+      <c r="D20" s="160">
+        <v>1</v>
+      </c>
       <c r="E20" s="164">
         <v>2</v>
       </c>
       <c r="F20" s="162"/>
-      <c r="G20" s="208">
+      <c r="G20" s="207">
         <v>2</v>
       </c>
-      <c r="H20" s="198"/>
-      <c r="I20" s="197"/>
-    </row>
-    <row r="21" spans="1:10" ht="15">
-      <c r="A21" s="209" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" s="187">
+      <c r="H20" s="197"/>
+      <c r="I20" s="196"/>
+    </row>
+    <row r="21" spans="1:11" ht="15">
+      <c r="A21" s="208" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="186">
         <f>SUMPRODUCT(B19:B20,C19:C20)</f>
         <v>4</v>
       </c>
@@ -7700,9 +7888,9 @@
         <f>SUM(C19:C20)</f>
         <v>4</v>
       </c>
-      <c r="D21" s="188">
+      <c r="D21" s="187">
         <f>SUMPRODUCT(D19:D20,E19:E20)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E21" s="166">
         <f>SUM(E19:E20)</f>
@@ -7712,31 +7900,31 @@
         <f>SUMPRODUCT(F19:F20,G19:G20)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="208">
+      <c r="G21" s="207">
         <f>SUM(G19:G20)</f>
         <v>4</v>
       </c>
-      <c r="H21" s="198"/>
-      <c r="I21" s="197"/>
-    </row>
-    <row r="22" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A22" s="317" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" s="318"/>
-      <c r="C22" s="318"/>
-      <c r="D22" s="318"/>
-      <c r="E22" s="318"/>
-      <c r="F22" s="318"/>
-      <c r="G22" s="319"/>
-      <c r="H22" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="I22" s="196"/>
-    </row>
-    <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="207" t="s">
-        <v>154</v>
+      <c r="H21" s="197"/>
+      <c r="I21" s="196"/>
+    </row>
+    <row r="22" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A22" s="316" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="317"/>
+      <c r="C22" s="317"/>
+      <c r="D22" s="317"/>
+      <c r="E22" s="317"/>
+      <c r="F22" s="317"/>
+      <c r="G22" s="318"/>
+      <c r="H22" s="195" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="195"/>
+    </row>
+    <row r="23" spans="1:11" ht="225">
+      <c r="A23" s="206" t="s">
+        <v>161</v>
       </c>
       <c r="B23" s="171">
         <v>0.75</v>
@@ -7744,23 +7932,28 @@
       <c r="C23" s="163">
         <v>4</v>
       </c>
-      <c r="D23" s="172"/>
+      <c r="D23" s="172">
+        <v>0.75</v>
+      </c>
       <c r="E23" s="164">
         <v>4</v>
       </c>
       <c r="F23" s="177"/>
-      <c r="G23" s="208">
+      <c r="G23" s="207">
         <v>4</v>
       </c>
-      <c r="H23" s="198"/>
-      <c r="I23" s="197"/>
+      <c r="H23" s="197"/>
+      <c r="I23" s="196"/>
       <c r="J23" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30">
-      <c r="A24" s="207" t="s">
-        <v>156</v>
+        <v>162</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30">
+      <c r="A24" s="206" t="s">
+        <v>164</v>
       </c>
       <c r="B24" s="171">
         <v>1</v>
@@ -7768,25 +7961,27 @@
       <c r="C24" s="163">
         <v>5</v>
       </c>
-      <c r="D24" s="172"/>
+      <c r="D24" s="172">
+        <v>1</v>
+      </c>
       <c r="E24" s="164">
         <v>5</v>
       </c>
       <c r="F24" s="177"/>
-      <c r="G24" s="208">
+      <c r="G24" s="207">
         <v>5</v>
       </c>
-      <c r="H24" s="198"/>
-      <c r="I24" s="197"/>
+      <c r="H24" s="197"/>
+      <c r="I24" s="196"/>
       <c r="J24" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15">
-      <c r="A25" s="209" t="s">
-        <v>143</v>
-      </c>
-      <c r="B25" s="187">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15">
+      <c r="A25" s="208" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="186">
         <f>SUMPRODUCT(B23:B24,C23:C24)</f>
         <v>8</v>
       </c>
@@ -7794,9 +7989,9 @@
         <f>SUM(C23:C24)</f>
         <v>9</v>
       </c>
-      <c r="D25" s="188">
+      <c r="D25" s="187">
         <f>SUMPRODUCT(D23:D24,E23:E24)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E25" s="166">
         <f>SUM(E23:E24)</f>
@@ -7806,31 +8001,31 @@
         <f>SUMPRODUCT(F23:F24,G23:G24)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="208">
+      <c r="G25" s="207">
         <f>SUM(G23:G24)</f>
         <v>9</v>
       </c>
-      <c r="H25" s="198"/>
-      <c r="I25" s="197"/>
-    </row>
-    <row r="26" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A26" s="317" t="s">
-        <v>158</v>
-      </c>
-      <c r="B26" s="318"/>
-      <c r="C26" s="318"/>
-      <c r="D26" s="318"/>
-      <c r="E26" s="318"/>
-      <c r="F26" s="318"/>
-      <c r="G26" s="319"/>
-      <c r="H26" s="196" t="s">
+      <c r="H25" s="197"/>
+      <c r="I25" s="196"/>
+    </row>
+    <row r="26" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A26" s="316" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26" s="317"/>
+      <c r="C26" s="317"/>
+      <c r="D26" s="317"/>
+      <c r="E26" s="317"/>
+      <c r="F26" s="317"/>
+      <c r="G26" s="318"/>
+      <c r="H26" s="195" t="s">
         <v>88</v>
       </c>
-      <c r="I26" s="196"/>
-    </row>
-    <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="203" t="s">
-        <v>159</v>
+      <c r="I26" s="195"/>
+    </row>
+    <row r="27" spans="1:11" ht="15">
+      <c r="A27" s="202" t="s">
+        <v>167</v>
       </c>
       <c r="B27" s="178">
         <v>1</v>
@@ -7838,20 +8033,22 @@
       <c r="C27" s="154">
         <v>2</v>
       </c>
-      <c r="D27" s="179"/>
+      <c r="D27" s="179">
+        <v>1</v>
+      </c>
       <c r="E27" s="156">
         <v>2</v>
       </c>
       <c r="F27" s="180"/>
-      <c r="G27" s="204">
+      <c r="G27" s="203">
         <v>2</v>
       </c>
-      <c r="H27" s="198"/>
-      <c r="I27" s="197"/>
-    </row>
-    <row r="28" spans="1:10" ht="120">
-      <c r="A28" s="205" t="s">
-        <v>160</v>
+      <c r="H27" s="197"/>
+      <c r="I27" s="196"/>
+    </row>
+    <row r="28" spans="1:11" ht="409.5">
+      <c r="A28" s="204" t="s">
+        <v>168</v>
       </c>
       <c r="B28" s="171">
         <v>0.5</v>
@@ -7859,23 +8056,25 @@
       <c r="C28" s="159">
         <v>3</v>
       </c>
-      <c r="D28" s="172"/>
+      <c r="D28" s="172">
+        <v>1</v>
+      </c>
       <c r="E28" s="161">
         <v>3</v>
       </c>
       <c r="F28" s="177"/>
-      <c r="G28" s="206">
+      <c r="G28" s="205">
         <v>3</v>
       </c>
-      <c r="H28" s="198"/>
-      <c r="I28" s="197"/>
+      <c r="H28" s="197"/>
+      <c r="I28" s="196"/>
       <c r="J28" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="30">
-      <c r="A29" s="207" t="s">
-        <v>162</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30">
+      <c r="A29" s="206" t="s">
+        <v>170</v>
       </c>
       <c r="B29" s="171">
         <v>1</v>
@@ -7883,20 +8082,22 @@
       <c r="C29" s="163">
         <v>3</v>
       </c>
-      <c r="D29" s="172"/>
+      <c r="D29" s="172">
+        <v>1</v>
+      </c>
       <c r="E29" s="164">
         <v>3</v>
       </c>
       <c r="F29" s="177"/>
-      <c r="G29" s="208">
+      <c r="G29" s="207">
         <v>3</v>
       </c>
-      <c r="H29" s="197"/>
-      <c r="I29" s="197"/>
-    </row>
-    <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="209" t="s">
-        <v>143</v>
+      <c r="H29" s="196"/>
+      <c r="I29" s="196"/>
+    </row>
+    <row r="30" spans="1:11" ht="15">
+      <c r="A30" s="208" t="s">
+        <v>150</v>
       </c>
       <c r="B30" s="181">
         <f>SUMPRODUCT(B27:B29,C27:C29)</f>
@@ -7908,7 +8109,7 @@
       </c>
       <c r="D30" s="182">
         <f>SUMPRODUCT(D27:D29,E27:E29)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E30" s="166">
         <f>SUM(E27:E29)</f>
@@ -7918,31 +8119,31 @@
         <f>SUMPRODUCT(F27:F29,G27:G29)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="208">
+      <c r="G30" s="207">
         <f>SUM(G27:G29)</f>
         <v>8</v>
       </c>
-      <c r="H30" s="198"/>
-      <c r="I30" s="197"/>
-    </row>
-    <row r="31" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A31" s="317" t="s">
-        <v>163</v>
-      </c>
-      <c r="B31" s="318"/>
-      <c r="C31" s="318"/>
-      <c r="D31" s="318"/>
-      <c r="E31" s="318"/>
-      <c r="F31" s="318"/>
-      <c r="G31" s="319"/>
-      <c r="H31" s="196" t="s">
+      <c r="H30" s="197"/>
+      <c r="I30" s="196"/>
+    </row>
+    <row r="31" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A31" s="316" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="317"/>
+      <c r="C31" s="317"/>
+      <c r="D31" s="317"/>
+      <c r="E31" s="317"/>
+      <c r="F31" s="317"/>
+      <c r="G31" s="318"/>
+      <c r="H31" s="195" t="s">
         <v>88</v>
       </c>
-      <c r="I31" s="196"/>
-    </row>
-    <row r="32" spans="1:10" ht="15">
-      <c r="A32" s="205" t="s">
-        <v>164</v>
+      <c r="I31" s="195"/>
+    </row>
+    <row r="32" spans="1:11" ht="15">
+      <c r="A32" s="204" t="s">
+        <v>172</v>
       </c>
       <c r="B32" s="171">
         <v>0.75</v>
@@ -7950,23 +8151,28 @@
       <c r="C32" s="159">
         <v>3</v>
       </c>
-      <c r="D32" s="172"/>
+      <c r="D32" s="172">
+        <v>0.75</v>
+      </c>
       <c r="E32" s="161">
         <v>3</v>
       </c>
       <c r="F32" s="177"/>
-      <c r="G32" s="206">
+      <c r="G32" s="205">
         <v>3</v>
       </c>
-      <c r="H32" s="197"/>
-      <c r="I32" s="197"/>
+      <c r="H32" s="196"/>
+      <c r="I32" s="196"/>
       <c r="J32" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="75">
-      <c r="A33" s="205" t="s">
-        <v>166</v>
+        <v>173</v>
+      </c>
+      <c r="K32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="345">
+      <c r="A33" s="204" t="s">
+        <v>175</v>
       </c>
       <c r="B33" s="171">
         <v>1</v>
@@ -7974,23 +8180,28 @@
       <c r="C33" s="159">
         <v>4</v>
       </c>
-      <c r="D33" s="172"/>
+      <c r="D33" s="172">
+        <v>0.75</v>
+      </c>
       <c r="E33" s="161">
         <v>4</v>
       </c>
       <c r="F33" s="177"/>
-      <c r="G33" s="206">
+      <c r="G33" s="205">
         <v>4</v>
       </c>
-      <c r="H33" s="197"/>
-      <c r="I33" s="197"/>
+      <c r="H33" s="196"/>
+      <c r="I33" s="196"/>
       <c r="J33" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="205" t="s">
-        <v>168</v>
+        <v>176</v>
+      </c>
+      <c r="K33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15">
+      <c r="A34" s="204" t="s">
+        <v>178</v>
       </c>
       <c r="B34" s="171">
         <v>1</v>
@@ -7998,20 +8209,22 @@
       <c r="C34" s="159">
         <v>3</v>
       </c>
-      <c r="D34" s="172"/>
+      <c r="D34" s="172">
+        <v>1</v>
+      </c>
       <c r="E34" s="161">
         <v>3</v>
       </c>
       <c r="F34" s="177"/>
-      <c r="G34" s="206">
+      <c r="G34" s="205">
         <v>3</v>
       </c>
-      <c r="H34" s="197"/>
-      <c r="I34" s="197"/>
-    </row>
-    <row r="35" spans="1:10" ht="15">
-      <c r="A35" s="205" t="s">
-        <v>169</v>
+      <c r="H34" s="196"/>
+      <c r="I34" s="196"/>
+    </row>
+    <row r="35" spans="1:11" ht="15">
+      <c r="A35" s="204" t="s">
+        <v>179</v>
       </c>
       <c r="B35" s="171">
         <v>1</v>
@@ -8019,20 +8232,22 @@
       <c r="C35" s="159">
         <v>4</v>
       </c>
-      <c r="D35" s="172"/>
+      <c r="D35" s="172">
+        <v>1</v>
+      </c>
       <c r="E35" s="161">
         <v>4</v>
       </c>
       <c r="F35" s="177"/>
-      <c r="G35" s="206">
+      <c r="G35" s="205">
         <v>4</v>
       </c>
-      <c r="H35" s="197"/>
-      <c r="I35" s="197"/>
-    </row>
-    <row r="36" spans="1:10" ht="15">
-      <c r="A36" s="205" t="s">
-        <v>170</v>
+      <c r="H35" s="196"/>
+      <c r="I35" s="196"/>
+    </row>
+    <row r="36" spans="1:11" ht="15">
+      <c r="A36" s="204" t="s">
+        <v>180</v>
       </c>
       <c r="B36" s="171">
         <v>1</v>
@@ -8040,20 +8255,22 @@
       <c r="C36" s="159">
         <v>4</v>
       </c>
-      <c r="D36" s="172"/>
+      <c r="D36" s="172">
+        <v>1</v>
+      </c>
       <c r="E36" s="161">
         <v>4</v>
       </c>
       <c r="F36" s="177"/>
-      <c r="G36" s="206">
+      <c r="G36" s="205">
         <v>4</v>
       </c>
-      <c r="H36" s="197"/>
-      <c r="I36" s="197"/>
-    </row>
-    <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="205" t="s">
-        <v>171</v>
+      <c r="H36" s="196"/>
+      <c r="I36" s="196"/>
+    </row>
+    <row r="37" spans="1:11" ht="15">
+      <c r="A37" s="204" t="s">
+        <v>181</v>
       </c>
       <c r="B37" s="171">
         <v>1</v>
@@ -8061,20 +8278,22 @@
       <c r="C37" s="159">
         <v>2</v>
       </c>
-      <c r="D37" s="172"/>
+      <c r="D37" s="172">
+        <v>1</v>
+      </c>
       <c r="E37" s="161">
         <v>2</v>
       </c>
       <c r="F37" s="177"/>
-      <c r="G37" s="206">
+      <c r="G37" s="205">
         <v>2</v>
       </c>
-      <c r="H37" s="197"/>
-      <c r="I37" s="197"/>
-    </row>
-    <row r="38" spans="1:10" ht="30">
-      <c r="A38" s="207" t="s">
-        <v>172</v>
+      <c r="H37" s="196"/>
+      <c r="I37" s="196"/>
+    </row>
+    <row r="38" spans="1:11" ht="30">
+      <c r="A38" s="206" t="s">
+        <v>182</v>
       </c>
       <c r="B38" s="171">
         <v>1</v>
@@ -8082,20 +8301,22 @@
       <c r="C38" s="163">
         <v>12</v>
       </c>
-      <c r="D38" s="172"/>
+      <c r="D38" s="172">
+        <v>1</v>
+      </c>
       <c r="E38" s="164">
         <v>12</v>
       </c>
       <c r="F38" s="177"/>
-      <c r="G38" s="208">
+      <c r="G38" s="207">
         <v>12</v>
       </c>
-      <c r="H38" s="197"/>
-      <c r="I38" s="197"/>
-    </row>
-    <row r="39" spans="1:10" ht="60">
-      <c r="A39" s="207" t="s">
-        <v>173</v>
+      <c r="H38" s="196"/>
+      <c r="I38" s="196"/>
+    </row>
+    <row r="39" spans="1:11" ht="409.5">
+      <c r="A39" s="206" t="s">
+        <v>183</v>
       </c>
       <c r="B39" s="171">
         <v>0.5</v>
@@ -8103,23 +8324,28 @@
       <c r="C39" s="163">
         <v>6</v>
       </c>
-      <c r="D39" s="172"/>
+      <c r="D39" s="172">
+        <v>0.25</v>
+      </c>
       <c r="E39" s="164">
         <v>6</v>
       </c>
       <c r="F39" s="177"/>
-      <c r="G39" s="208">
+      <c r="G39" s="207">
         <v>6</v>
       </c>
-      <c r="H39" s="197"/>
-      <c r="I39" s="197"/>
+      <c r="H39" s="196"/>
+      <c r="I39" s="196"/>
       <c r="J39" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15">
-      <c r="A40" s="207" t="s">
-        <v>175</v>
+        <v>184</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15">
+      <c r="A40" s="206" t="s">
+        <v>186</v>
       </c>
       <c r="B40" s="171">
         <v>1</v>
@@ -8127,20 +8353,22 @@
       <c r="C40" s="163">
         <v>3</v>
       </c>
-      <c r="D40" s="172"/>
+      <c r="D40" s="172">
+        <v>1</v>
+      </c>
       <c r="E40" s="164">
         <v>3</v>
       </c>
       <c r="F40" s="177"/>
-      <c r="G40" s="208">
+      <c r="G40" s="207">
         <v>3</v>
       </c>
-      <c r="H40" s="197"/>
-      <c r="I40" s="197"/>
-    </row>
-    <row r="41" spans="1:10" ht="150">
-      <c r="A41" s="209" t="s">
-        <v>143</v>
+      <c r="H40" s="196"/>
+      <c r="I40" s="196"/>
+    </row>
+    <row r="41" spans="1:11" ht="409.5">
+      <c r="A41" s="208" t="s">
+        <v>150</v>
       </c>
       <c r="B41" s="181">
         <f>SUMPRODUCT(B32:B40,C32:C40)</f>
@@ -8152,7 +8380,7 @@
       </c>
       <c r="D41" s="182">
         <f>SUMPRODUCT(D32:D40,E32:E40)</f>
-        <v>0</v>
+        <v>34.75</v>
       </c>
       <c r="E41" s="166">
         <f>SUM(E32:E40)</f>
@@ -8162,34 +8390,34 @@
         <f>SUMPRODUCT(F32:F40,G32:G40)</f>
         <v>0</v>
       </c>
-      <c r="G41" s="208">
+      <c r="G41" s="207">
         <f>SUM(G32:G40)</f>
         <v>41</v>
       </c>
-      <c r="H41" s="198"/>
-      <c r="I41" s="197"/>
+      <c r="H41" s="197"/>
+      <c r="I41" s="196"/>
       <c r="J41" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A42" s="317" t="s">
-        <v>177</v>
-      </c>
-      <c r="B42" s="318"/>
-      <c r="C42" s="318"/>
-      <c r="D42" s="318"/>
-      <c r="E42" s="318"/>
-      <c r="F42" s="318"/>
-      <c r="G42" s="319"/>
-      <c r="H42" s="196" t="s">
-        <v>96</v>
-      </c>
-      <c r="I42" s="196"/>
-    </row>
-    <row r="43" spans="1:10" ht="30">
-      <c r="A43" s="210" t="s">
-        <v>178</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A42" s="316" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" s="317"/>
+      <c r="C42" s="317"/>
+      <c r="D42" s="317"/>
+      <c r="E42" s="317"/>
+      <c r="F42" s="317"/>
+      <c r="G42" s="318"/>
+      <c r="H42" s="195" t="s">
+        <v>90</v>
+      </c>
+      <c r="I42" s="195"/>
+    </row>
+    <row r="43" spans="1:11" ht="30">
+      <c r="A43" s="209" t="s">
+        <v>189</v>
       </c>
       <c r="B43" s="178">
         <v>1</v>
@@ -8197,20 +8425,22 @@
       <c r="C43" s="183">
         <v>3</v>
       </c>
-      <c r="D43" s="179"/>
+      <c r="D43" s="179">
+        <v>1</v>
+      </c>
       <c r="E43" s="184">
         <v>3</v>
       </c>
       <c r="F43" s="180"/>
-      <c r="G43" s="211">
+      <c r="G43" s="210">
         <v>3</v>
       </c>
-      <c r="H43" s="198"/>
-      <c r="I43" s="197"/>
-    </row>
-    <row r="44" spans="1:10" ht="30">
-      <c r="A44" s="207" t="s">
-        <v>179</v>
+      <c r="H43" s="197"/>
+      <c r="I43" s="196"/>
+    </row>
+    <row r="44" spans="1:11" ht="30">
+      <c r="A44" s="206" t="s">
+        <v>190</v>
       </c>
       <c r="B44" s="171">
         <v>1</v>
@@ -8218,46 +8448,50 @@
       <c r="C44" s="163">
         <v>4</v>
       </c>
-      <c r="D44" s="172"/>
+      <c r="D44" s="172">
+        <v>1</v>
+      </c>
       <c r="E44" s="164">
         <v>4</v>
       </c>
       <c r="F44" s="177"/>
-      <c r="G44" s="208">
+      <c r="G44" s="207">
         <v>4</v>
       </c>
-      <c r="H44" s="197"/>
-      <c r="I44" s="197"/>
+      <c r="H44" s="196"/>
+      <c r="I44" s="196"/>
       <c r="J44" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="45">
-      <c r="A45" s="205" t="s">
-        <v>181</v>
-      </c>
-      <c r="B45" s="284">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="45">
+      <c r="A45" s="204" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" s="283">
         <v>1</v>
       </c>
       <c r="C45" s="159">
         <v>4</v>
       </c>
-      <c r="D45" s="185"/>
+      <c r="D45" s="329">
+        <v>1</v>
+      </c>
       <c r="E45" s="161">
         <v>4</v>
       </c>
-      <c r="F45" s="186"/>
-      <c r="G45" s="206">
+      <c r="F45" s="185"/>
+      <c r="G45" s="205">
         <v>4</v>
       </c>
-      <c r="H45" s="199"/>
-      <c r="I45" s="197"/>
-    </row>
-    <row r="46" spans="1:10" ht="15">
-      <c r="A46" s="212" t="s">
-        <v>143</v>
-      </c>
-      <c r="B46" s="187">
+      <c r="H45" s="198"/>
+      <c r="I45" s="196"/>
+    </row>
+    <row r="46" spans="1:11" ht="15">
+      <c r="A46" s="211" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="186">
         <f>SUMPRODUCT(B43:B45,C43:C45)</f>
         <v>11</v>
       </c>
@@ -8265,114 +8499,114 @@
         <f>SUM(C43:C45)</f>
         <v>11</v>
       </c>
-      <c r="D46" s="188">
+      <c r="D46" s="187">
         <f>SUMPRODUCT(D43:D45,E43:E45)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E46" s="166">
         <f>SUM(E43:E45)</f>
         <v>11</v>
       </c>
-      <c r="F46" s="189">
+      <c r="F46" s="188">
         <f>SUMPRODUCT(F43:F45,G43:G45)</f>
         <v>0</v>
       </c>
-      <c r="G46" s="213">
+      <c r="G46" s="212">
         <f>SUM(G43:G45)</f>
         <v>11</v>
       </c>
-      <c r="H46" s="197"/>
-      <c r="I46" s="197"/>
-    </row>
-    <row r="47" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A47" s="317" t="s">
+      <c r="H46" s="196"/>
+      <c r="I46" s="196"/>
+    </row>
+    <row r="47" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A47" s="316" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="318"/>
-      <c r="C47" s="318"/>
-      <c r="D47" s="318"/>
-      <c r="E47" s="318"/>
-      <c r="F47" s="318"/>
-      <c r="G47" s="319"/>
-      <c r="H47" s="196"/>
-      <c r="I47" s="196"/>
-    </row>
-    <row r="48" spans="1:10" ht="15">
-      <c r="A48" s="214" t="s">
-        <v>182</v>
-      </c>
-      <c r="B48" s="190">
+      <c r="B47" s="317"/>
+      <c r="C47" s="317"/>
+      <c r="D47" s="317"/>
+      <c r="E47" s="317"/>
+      <c r="F47" s="317"/>
+      <c r="G47" s="318"/>
+      <c r="H47" s="195"/>
+      <c r="I47" s="195"/>
+    </row>
+    <row r="48" spans="1:11" ht="15">
+      <c r="A48" s="213" t="s">
+        <v>193</v>
+      </c>
+      <c r="B48" s="189">
         <f t="shared" ref="B48:G48" si="0">B11+B17+B21+B25+B30+B41+B46</f>
         <v>92.75</v>
       </c>
-      <c r="C48" s="191">
+      <c r="C48" s="190">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="D48" s="192">
+      <c r="D48" s="191">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E48" s="193">
+        <v>90.75</v>
+      </c>
+      <c r="E48" s="192">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F48" s="194">
+      <c r="F48" s="193">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G48" s="215">
+      <c r="G48" s="214">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H48" s="199"/>
-      <c r="I48" s="197"/>
+      <c r="H48" s="198"/>
+      <c r="I48" s="196"/>
     </row>
     <row r="49" spans="1:9" ht="15">
-      <c r="A49" s="216" t="s">
-        <v>183</v>
-      </c>
-      <c r="B49" s="326">
+      <c r="A49" s="215" t="s">
+        <v>194</v>
+      </c>
+      <c r="B49" s="325">
         <f>B48/C48</f>
         <v>0.92749999999999999</v>
       </c>
-      <c r="C49" s="326"/>
-      <c r="D49" s="327">
+      <c r="C49" s="325"/>
+      <c r="D49" s="326">
         <f>D48/E48</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="327"/>
-      <c r="F49" s="328">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="E49" s="326"/>
+      <c r="F49" s="327">
         <f>F48/G48</f>
         <v>0</v>
       </c>
-      <c r="G49" s="329"/>
-      <c r="H49" s="201"/>
-      <c r="I49" s="201"/>
+      <c r="G49" s="328"/>
+      <c r="H49" s="200"/>
+      <c r="I49" s="200"/>
     </row>
     <row r="50" spans="1:9" ht="15">
-      <c r="H50" s="200"/>
-      <c r="I50" s="200"/>
+      <c r="H50" s="199"/>
+      <c r="I50" s="199"/>
     </row>
     <row r="51" spans="1:9" ht="15">
-      <c r="H51" s="200"/>
-      <c r="I51" s="200"/>
+      <c r="H51" s="199"/>
+      <c r="I51" s="199"/>
     </row>
     <row r="52" spans="1:9" ht="15">
-      <c r="H52" s="200"/>
-      <c r="I52" s="200"/>
+      <c r="H52" s="199"/>
+      <c r="I52" s="199"/>
     </row>
     <row r="53" spans="1:9" ht="15">
-      <c r="H53" s="200"/>
-      <c r="I53" s="200"/>
+      <c r="H53" s="199"/>
+      <c r="I53" s="199"/>
     </row>
     <row r="54" spans="1:9" ht="15">
-      <c r="H54" s="200"/>
-      <c r="I54" s="200"/>
+      <c r="H54" s="199"/>
+      <c r="I54" s="199"/>
     </row>
     <row r="55" spans="1:9" ht="15">
-      <c r="H55" s="200"/>
-      <c r="I55" s="200"/>
+      <c r="H55" s="199"/>
+      <c r="I55" s="199"/>
     </row>
     <row r="56" spans="1:9" ht="15"/>
     <row r="57" spans="1:9" ht="15"/>
@@ -8403,7 +8637,7 @@
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Les évaluations sont faites en terme de pourcentage. Veuillez entrer une valeur entre 0 et 1" sqref="B8:B10 D8:D10 F8:F10 H8:H10 B13:B16 D13:D16 F13:F16 H13:H16 B27:B29 D27:D29 F27:F29 H27:H29 B32:B40 D32:D40 F32:F40 H32:H40 B43:B45 D43:D45 F43:F45 H43:H45 H19:H20 F19:F20 D19:D20 B19:B20 H23:H24 F23:F24 D23:D24 B23:B24" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Les évaluations sont faites en terme de pourcentage. Veuillez entrer une valeur entre 0 et 1" sqref="B8:B10 D8:D10 F8:F10 H8:H10 B13:B16 D13:D16 F13:F16 H13:H16 B27:B29 D27:D29 F27:F29 H27:H29 B32:B40 D32:D40 F32:F40 H32:H40 B43:B45 B23:B24 F43:F45 H43:H45 H19:H20 F19:F20 D19:D20 B19:B20 H23:H24 F23:F24 D23:D24 D43:D44" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -8449,7 +8683,7 @@
       <c r="F2" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="290" t="s">
+      <c r="G2" s="289" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8462,11 +8696,11 @@
       <c r="D3" s="55"/>
       <c r="E3" s="56"/>
       <c r="F3" s="57"/>
-      <c r="G3" s="290"/>
+      <c r="G3" s="289"/>
     </row>
     <row r="4" spans="1:7" ht="30">
       <c r="A4" s="58" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="60"/>
@@ -8492,7 +8726,7 @@
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="65" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="B6" s="66"/>
       <c r="C6" s="67"/>
@@ -8505,7 +8739,7 @@
     </row>
     <row r="7" spans="1:7" ht="15">
       <c r="A7" s="65" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="B7" s="66"/>
       <c r="C7" s="67"/>
@@ -8518,7 +8752,7 @@
     </row>
     <row r="8" spans="1:7" ht="30">
       <c r="A8" s="65" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="B8" s="66"/>
       <c r="C8" s="67"/>
@@ -8531,7 +8765,7 @@
     </row>
     <row r="9" spans="1:7" ht="15">
       <c r="A9" s="65" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="B9" s="66"/>
       <c r="C9" s="67"/>
@@ -8544,7 +8778,7 @@
     </row>
     <row r="10" spans="1:7" ht="30">
       <c r="A10" s="65" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="B10" s="66"/>
       <c r="C10" s="67"/>
@@ -8557,7 +8791,7 @@
     </row>
     <row r="11" spans="1:7" ht="30">
       <c r="A11" s="65" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B11" s="66"/>
       <c r="C11" s="67"/>
@@ -8570,7 +8804,7 @@
     </row>
     <row r="12" spans="1:7" ht="15">
       <c r="A12" s="65" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="B12" s="66"/>
       <c r="C12" s="67"/>
@@ -8583,7 +8817,7 @@
     </row>
     <row r="13" spans="1:7" ht="30">
       <c r="A13" s="65" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B13" s="66"/>
       <c r="C13" s="67"/>
@@ -8596,7 +8830,7 @@
     </row>
     <row r="14" spans="1:7" ht="15">
       <c r="A14" s="65" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B14" s="66"/>
       <c r="C14" s="67"/>
@@ -8609,7 +8843,7 @@
     </row>
     <row r="15" spans="1:7" ht="15">
       <c r="A15" s="65" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="B15" s="66"/>
       <c r="C15" s="67"/>
@@ -8622,7 +8856,7 @@
     </row>
     <row r="16" spans="1:7" ht="15">
       <c r="A16" s="65" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="B16" s="66"/>
       <c r="C16" s="67"/>
@@ -8635,7 +8869,7 @@
     </row>
     <row r="17" spans="1:7" ht="15">
       <c r="A17" s="65" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="B17" s="66"/>
       <c r="C17" s="67"/>
@@ -8648,7 +8882,7 @@
     </row>
     <row r="18" spans="1:7" ht="30">
       <c r="A18" s="65" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="B18" s="66"/>
       <c r="C18" s="67"/>
@@ -8661,7 +8895,7 @@
     </row>
     <row r="19" spans="1:7" ht="15">
       <c r="A19" s="65" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="B19" s="66"/>
       <c r="C19" s="67"/>
@@ -8674,7 +8908,7 @@
     </row>
     <row r="20" spans="1:7" ht="15">
       <c r="A20" s="65" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="B20" s="66"/>
       <c r="C20" s="67"/>
@@ -8687,7 +8921,7 @@
     </row>
     <row r="21" spans="1:7" ht="45">
       <c r="A21" s="65" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="B21" s="66"/>
       <c r="C21" s="67"/>
@@ -8700,7 +8934,7 @@
     </row>
     <row r="22" spans="1:7" ht="15">
       <c r="A22" s="65" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="B22" s="66"/>
       <c r="C22" s="67"/>
@@ -8713,7 +8947,7 @@
     </row>
     <row r="23" spans="1:7" ht="30">
       <c r="A23" s="65" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="B23" s="66"/>
       <c r="C23" s="67"/>
@@ -8726,7 +8960,7 @@
     </row>
     <row r="24" spans="1:7" ht="15">
       <c r="A24" s="65" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="B24" s="66"/>
       <c r="C24" s="67"/>
@@ -8739,7 +8973,7 @@
     </row>
     <row r="25" spans="1:7" ht="15">
       <c r="A25" s="65" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="B25" s="66"/>
       <c r="C25" s="67"/>
@@ -8752,7 +8986,7 @@
     </row>
     <row r="26" spans="1:7" ht="30">
       <c r="A26" s="65" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="B26" s="66"/>
       <c r="C26" s="67"/>
@@ -8765,7 +8999,7 @@
     </row>
     <row r="27" spans="1:7" ht="30">
       <c r="A27" s="72" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="B27" s="73"/>
       <c r="C27" s="74"/>
@@ -8862,10 +9096,10 @@
       <c r="D33" s="85"/>
       <c r="E33" s="85"/>
       <c r="F33" s="85"/>
-      <c r="H33" s="291" t="s">
+      <c r="H33" s="290" t="s">
         <v>55</v>
       </c>
-      <c r="I33" s="291"/>
+      <c r="I33" s="290"/>
     </row>
     <row r="34" spans="1:9" ht="15">
       <c r="A34" s="52" t="s">
@@ -9115,7 +9349,7 @@
     <row r="49" spans="1:6" ht="15"/>
     <row r="50" spans="1:6" ht="15">
       <c r="A50" s="92" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="B50" s="139">
         <f>(B$31+B$47)/2</f>

</xml_diff>